<commit_message>
Fixed Next Scheduled Dose Order Example.
</commit_message>
<xml_diff>
--- a/output/nswhealthitocmedicationadministration.xlsx
+++ b/output/nswhealthitocmedicationadministration.xlsx
@@ -968,7 +968,7 @@
 </t>
   </si>
   <si>
-    <t>The practioner(s) who performed the administration.</t>
+    <t>Who performed the medication administration and what they did</t>
   </si>
   <si>
     <t>Indicates who or what performed the medication administration and how they were involved.</t>
@@ -10334,7 +10334,7 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F78" t="s" s="2">
         <v>43</v>

</xml_diff>